<commit_message>
15 | Day 3
</commit_message>
<xml_diff>
--- a/Batch/15/Curriculum/Day_3_Arithmetic.xlsx
+++ b/Batch/15/Curriculum/Day_3_Arithmetic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28422"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\14\Curriculum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\15\Curriculum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1C3B39-88C5-4FBE-963A-88F4588EE8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D50E60-3A80-46F7-9566-6F14857CEA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="750" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goal" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="86">
   <si>
     <r>
       <rPr>
@@ -329,20 +329,30 @@
   <si>
     <t>=SUMIFS(C6:C9,C6:C9,"&gt;100",C6:C9,"&lt;500")</t>
   </si>
+  <si>
+    <t>Acciojob</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -416,7 +426,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,6 +443,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -587,132 +603,136 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="38" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{E13C9D41-D07F-4CD3-A10A-1D1D5AF155F3}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -877,201 +897,6 @@
     </xdr:pic>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>55414</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>49691</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>131816</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>161291</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="6" name="Ink 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33A4DB48-8140-5A80-43F2-5AFFDACC297A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="3496320" y="942660"/>
-            <a:ext cx="76402" cy="111600"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="6" name="Ink 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33A4DB48-8140-5A80-43F2-5AFFDACC297A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3489793" y="936540"/>
-              <a:ext cx="89456" cy="123840"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76376</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>20219</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>542576</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152699</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="9" name="Ink 8">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D4D4AB-3F16-F645-EB9E-19242A636FC1}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="3517282" y="1091782"/>
-            <a:ext cx="466200" cy="132480"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="9" name="Ink 8">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D4D4AB-3F16-F645-EB9E-19242A636FC1}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3511095" y="1085662"/>
-              <a:ext cx="478574" cy="144720"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>45694</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>154091</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>478282</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>173512</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="29" name="Ink 28">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9025947-541C-F182-1E30-7FD99AA202BC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="3486600" y="1047060"/>
-            <a:ext cx="2325682" cy="555202"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="29" name="Ink 28">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9025947-541C-F182-1E30-7FD99AA202BC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3480466" y="1040931"/>
-              <a:ext cx="2337949" cy="567460"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1309,110 +1134,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2024-11-16T16:12:19.724"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#F6630D"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">184 84 1953,'0'0'8759,"2"-10"-7623,2-1-713,-2 7-160,-1-1 1,1 0 0,-1 1-1,0-1 1,-1 1 0,1-1-1,-1-9 847,-15 24-756,-13 23-326,2 1 0,2 1 0,-38 71 0,28-46-25,25-45-1786,11-22-2904,5-11 3314,1-5-327,-2-4-866</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="199.75">184 84 3650</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="387.29">184 84 3650,'-116'-48'1961,"70"22"1284,33 16-1408,22 18-1596,0 0 1,0 0-1,-1 1 0,12 16 1,6 6-6,-1 2-8,-21-27-113,0-1 0,0 1 0,0-1 0,0 0 0,1 0 0,0 0 0,9 6-1,-14-10 631,5 11-1587,-5-2-3343,0-5-126</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2024-11-16T16:12:30.555"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#F6630D"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">17 286 3490,'0'0'5071,"-15"-16"6,15 31-5076,-1 23 27,1-37-28,0 1 1,0-1-1,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 1,0 0-1,1 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 1,0 0-1,0 1 0,0-1 0,1 1 0,0-1 5,-1-1 0,1 1 0,-1-1 0,1 0 0,0 0-1,-1 1 1,1-1 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1 0-1,0-1 1,-1 1 0,1 0 0,-1-1 0,1 0 0,-1 1 0,1-1-1,-1 0 1,0 0 0,1 0 0,-1 0 0,2-1 0,36-35-28,-24 21 18,75-52-94,-63 50 73,-2-2 0,0 0 0,26-28 0,-44 41-44,-6 9-626,-9 15-1713,4-9 1003,-1 2-2276</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1869.11">501 215 5475,'0'0'4647,"0"-3"-3068,0 5-239,2 6-1326,0 0 0,1 0-1,0-1 1,1 1 0,-1-1 0,1 1 0,1-1 0,-1 0 0,9 9 0,8 16 28,-19-29-10,0 1 0,0-1 0,0 1 0,0-1 0,1 0 0,-1 0 0,1 0 0,0-1 0,4 5 0,-5-7 2,-1 1 0,1-1 0,0 1-1,-1-1 1,1 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1 0-1,1 0 1,-1 0 0,1-1-1,0 1 1,-1-1 0,1 1 0,-1-1-1,1 1 1,-1-1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,2-2-1,365-207 55,-148 93-72,-166 90 24,-50 26-40,-3 1-32,-1 2-248,-1-1 135,1 1 0,0 0 1,-1 0-1,1 0 0,-1-1 1,1 1-1,-1 0 1,0-1-1,0 1 0,0 0 1,0-1-1,-2 3 0,-11 14-1880,-5-1-1115</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2024-11-16T16:12:35.003"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#F6630D"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">60 878 6195,'0'0'4487,"0"8"-1323,43 42-3116,-42-49-30,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,2 0 0,-1 0-11,1-1 1,-1 1 0,0-1 0,1 0 0,-1 0-1,0 0 1,0-1 0,0 1 0,3-4-1,-5 5 23,-1-5 923</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1117.29">34 893 4866,'0'0'5144,"25"22"-4325,-8 4 127,-13-20-800,-1-1 1,1 1-1,0-1 0,0 1 0,1-1 1,-1-1-1,1 1 0,0 0 1,6 3-1,-10-9-7,-1 0-1,0-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1 1 1,1-1-1,0 0 0,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,2-2-1,37-24-513,-34 23 550,66-40-155,-42 27-3,1-2 0,-2-1 0,52-46 0,-72 54-16,16-11-4,-24 21-13,3 1-32,-4 0-147,-3 20-4615,-13-6 661</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2841.72">761 878 5282,'0'0'5123,"-14"-2"-502,14 6-4620,0 0 1,0 0-1,1 1 1,0-1-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0-1 1,1 1-1,3 3 1,12 20 16,-16-22-2,0 0 0,0 0 0,-1 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,0 6 1457,13-14-1436,-1 0 0,0 0 0,0-2-1,0 1 1,0-2 0,-1 1 0,21-13 0,4 0-15,82-41 14,141-93 0,-256 149-36,20-13-3,0 1-1,1 1 0,1 1 0,0 1 0,0 1 1,29-7-1,-54 17-80,0 0 1,0 0-1,0 0 0,1-1 1,-1 1-1,0 0 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,0 0 1,1 0-1,-1-1 0,0 1 1,0 0-1,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,0 1 1,1-1-1,-1 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,0 0 1,0 0-1,1 1 0,-1-1 1,0 0-1,0 0 0,0 0 1,0 1-1,1-1 1,-1 0-1,0 0 0,0 0 1,0 1-1,0-1 1,0 0-1,0 0 0,0 0 1,1 1-1,-1-1 0,0 0 1,0 0-1,0 1 1,0-1-1,0 0 0,0 0 1,0 1-1,0-1 0,-1 0 1,-3 6-3140</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5115.51">11 1367 7523,'0'0'5048,"-1"0"-4904,1 0-1,-1 1 1,0-1-1,1 1 1,-1-1 0,1 1-1,-1-1 1,1 1-1,-1-1 1,1 1-1,-1 0 1,1-1 0,-1 1-1,1-1 1,0 1-1,-1 0 1,1 0 0,0-1-1,0 1 1,-1 0-1,1 1 1,0 5-141,0 0 0,0 1 0,1-1 0,0 0 0,0 0 0,1 0 0,0 1 0,5 12 0,-6-16 8,-1-4-9,0 1 1,0 0-1,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,1 1 1,-1-1-1,0 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1-1 0,0 0 1,1 1-1,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 0 1,1 1-1,-1-1 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,1 0 1,-2 0-6,30 0 211,-18-2-195,0-1 0,0 0-1,-1 0 1,1-2 0,-1 1 0,0-1-1,0-1 1,19-13 0,4-1 13,7-1 13,-1-2 0,-1-2 0,-1-1 0,37-34 0,-27 27 49,-47 32-173</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6424.45">1242 1259 7668,'0'0'5357,"-6"-4"-4856,2 2-458,3 1-20,-1-1 0,0 1 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,-1 1 1,1-1-1,0 1 1,0-1-1,0 1 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 1 0,-1-1 1,1 1-1,0 0 1,-3 1-1,-21 23 225,1 1 0,0 0-1,2 2 1,-31 50 0,-7 8 79,36-62-5198,25-40 1242</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6810.1">937 1267 6259,'0'0'3972,"15"7"-3203,202 167 1923,-189-151-2527,33 32 297,-60-53-308</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8333.29">1819 159 480,'0'0'10173,"-3"-6"-9045,-1-2-1175,3 5 177,1 0 1,-2 0-1,1 1 0,0-1 0,0 0 0,-1 1 0,0 0 0,1-1 1,-1 1-1,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,0 1-1,-1-1 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1 0 1,0 0-1,0 1 0,0-1 0,1 1 0,-1-1 0,-5 1 0,6 1-130,0-1-1,1 1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 1 1,1-1-1,0 0 0,-1 1 1,1-1-1,0 1 1,0-1-1,-1 1 0,1-1 1,1 1-1,-1 0 1,0 0-1,0-1 0,0 4 1,-15 39-1,16-44 1,-5 25 21,0 0 0,2 0 0,-1 27 0,-3 30 47,1-27 77,2 67 0,3-65-98,-8 60 0,2-38 68,4 129 0,3-119-54,0-87-55,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 0-1,1 0 1,0-1 0,0 1 0,0 0 0,0 0-1,0-1 1,0 1 0,1 0 0,-1-1-1,1 0 1,-1 1 0,1-1 0,-1 0-1,1 0 1,0 1 0,-1-1 0,1 0-1,3 1 1,3 0 32,0-1-1,0 1 1,0-1-1,1 0 1,14-1 0,-20 0-39,1-1 6,0 0 0,0 0 1,-1 0-1,1 0 0,0-1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,0-1 0,0 1 0,0-1 1,4-3-1,37-40 33,-30 27-79,0 0 1,-1 0 0,-1-1 0,0-1 0,-2 0-1,0-1 1,9-34 0,-10 23-115,-2-1 0,-2 0 0,-1 0 0,-1-53 0,-4 20 89,-3-1-1,-19-103 0,19 152 64,0-7 27,0 1 0,-2-1 1,-1 1-1,-1 0 1,-2 1-1,0 0 1,-16-27-1,26 50-46,-1 1 0,1 0 1,0 0-1,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 1,0 0-1,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 1 1,0-1-1,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 1 0,0-1 1,0 0-1,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,1-1 0,-6 22-1128,4 4-1026,1 0-1794</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9030.16">2672 251 800,'0'0'11779,"-3"-17"-10941,-5-53-32,8 66-741,0-1 1,0 1-1,1 0 0,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,1 0-1,0 1 1,0-1-1,0 1 1,0-1-1,1 1 1,-1 0-1,1-1 1,0 1-1,0 1 1,0-1-1,1 0 1,-1 1-1,0 0 1,1-1-1,0 2 1,-1-1-1,1 0 1,0 1-1,0-1 1,0 1-1,0 0 1,0 0-1,0 1 1,1-1-1,-1 1 1,0 0-1,0 0 1,0 1-1,0-1 1,5 2-1,-7-1-63,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0 2 1,-5 56 16,1-48-9,0 0-1,-2 0 1,0 0-1,0 0 1,-1-1-1,0 0 1,-1-1-1,-1 0 1,0 0-1,-19 18 0,-13 9-347,-59 41-1,97-76 296,-17 12-198,15-10 102,-1 0 0,1 0 0,-1 0 0,-1-1 1,1 0-1,-1-1 0,1 1 0,-1-1 0,0 0 0,0-1 1,-1 0-1,-8 2 0,23-28-272,0 16 441,0 1 0,1 0 0,0 1 0,0 0 0,0 0 0,1 0 0,0 1 0,0 1 0,0-1 0,1 2 0,-1-1 1,1 1-1,0 1 0,0-1 0,0 2 0,0-1 0,0 2 0,0-1 0,1 1 0,18 3 0,-22-2 18,0 0-1,0 0 1,0 1 0,0 0 0,0 0-1,-1 0 1,1 1 0,-1 0-1,1 1 1,-1-1 0,0 1 0,0 0-1,-1 1 1,1-1 0,-1 1-1,0 0 1,0 1 0,-1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,-1 1-1,0-1 1,0 1 0,-1 0-1,0-1 1,0 1 0,-1 0 0,1 10-1,-1 0-248,-1-13-148,0 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,0 0 0,1 0 0,-1 0 0,3 4 0,5 0-3887</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9416.57">3018 286 8132,'0'0'6781,"-7"3"-6679,5-1-94,-1-1 0,1 1 1,-1-1-1,1 1 0,0 0 1,0-1-1,0 1 0,0 0 1,0 1-1,0-1 0,0 0 0,1 0 1,-1 1-1,1-1 0,-1 1 1,1 0-1,-1 2 0,0 4 22,0 0 1,1 0-1,0 0 0,0 0 0,1 10 1,0-18-30,0 0 0,1 0 1,-1 0-1,0 0 1,0 0-1,1-1 0,-1 1 1,0 0-1,1 0 0,-1-1 1,1 1-1,-1 0 1,1 0-1,-1-1 0,1 1 1,-1 0-1,1-1 0,0 1 1,-1-1-1,1 1 1,0-1-1,0 1 0,-1-1 1,1 0-1,0 1 0,1-1 1,31 6 80,-29-6-70,-1 0 0,1 0 0,0 0 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,6-4-1,-6-1 9,-1 0-1,0 0 1,0 0-1,0-1 0,-1 1 1,0-1-1,0 0 0,-1 1 1,0-1-1,0 0 1,-2-12-1,0-10 127,2 29-148,1-1-1,-1 1 1,0 0-1,0-1 0,0 1 1,0-1-1,0 1 0,0-1 1,-1 1-1,1 0 1,0-1-1,-1 1 0,1-1 1,-1 1-1,1 0 1,-1 0-1,0-1 0,0 1 1,1 0-1,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,0 1-1,-1-1 0,1 0 1,0 1-1,-1-1 1,1 1-1,0 0 0,-1-1 1,1 1-1,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,-1 0 1,-2 1-1,3 0-50,-1-1 0,1 1 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 0 0,0 1 1,0-1-1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 1,1 0-1,-1-1 0,1 1 0,-1 0 0,1 0 0,0-1 1,-1 4-1,1-3-272,-1 0 0,1 0 1,-1 0-1,1 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 1,-1-1-1,1 1 0,-1 0 1,1 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0-1-1,0 1 0,0-1 1,0 1-1,3 1 0,18 4-5424</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9739.07">3231 297 6979,'0'0'5467,"0"9"-4824,-1 8-263,-1-4-137,1-1 1,1 0-1,0 1 1,1-1-1,3 17 1,-4-28-233,1-1 1,0 1 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 0-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,2-1 0,25-8 202,-24 5-197,0 0 0,-1 0 1,0-1-1,1 1 0,-2-1 0,1 0 1,-1 0-1,1 0 0,-1 0 0,-1 0 1,1 0-1,-1-1 0,0 1 0,0-1 1,0 1-1,-1-1 0,0 1 1,0 0-1,-1-10 0,0 12 3,1 0 1,0 0-1,-1-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,0 0 0,1 0 1,-1 1-1,0-1 1,0 1-1,-1-1 0,1 1 1,0 0-1,-1 0 0,0 0 1,1 0-1,-1 0 1,0 0-1,0 1 0,0 0 1,0-1-1,0 1 0,0 0 1,0 1-1,0-1 0,-1 0 1,1 1-1,-4 0 1,5-1-33,0 1 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 1 0,0-1 1,0 1-1,0-1 1,0 1-1,0-1 0,0 1 1,0 0-1,1 0 1,-1 0-1,0 0 0,1 0 1,-1 1-1,1-1 1,-3 3-1,2 0-145,0-1-1,0 1 1,1 0 0,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,1 7 0,0 43-4541,9-31 288</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10039.23">3520 376 9989,'0'0'6234,"-4"-2"-5793,4 2-437,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,0-1 1,-1 1 0,1 0-1,0 0 1,0 0 0,-1-1-1,1 1 1,0 0 0,0 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0-1-1,-1 1 1,1 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0 0 0,1 0-1,-1-1 1,0 1 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,1-1 0,-1 1-1,0 0 1,0 0 0,0-1-1,1 1 1,-1 0 0,0 0-1,0 0 1,1-1 0,28-14 96,57-12-55,-72 23-8,121-32-860,-134 36-120,-7 5-3588,-11 2 2908,14-5 531,-24 9-3724</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10268.31">3606 204 7395,'0'0'7468,"0"-1"-7460,-1 1-1,1 0 1,0-1 0,-1 1-1,1 0 1,0 0 0,-1-1 0,1 1-1,-1 0 1,1 0 0,0 0 0,-1 0-1,1 0 1,-1-1 0,1 1 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,-1 1-1,1-1 1,-1 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,-1 1 0,1-1-1,-1 0 1,1 0 0,0 1 0,-1-1-1,1 0 1,0 1 0,-1-1 0,1 1-1,-3 8 63,1 1 1,0-1-1,0 0 0,1 1 0,1 0 0,0-1 0,1 16 0,-1 10 303,-14 204 334,14-238-817,-1 0 0,1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 1,0 1-1,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 1,0-1-1,1 1 0,-1-1 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 1 0,3-1 0,20 0-5746</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10661.79">3861 170 10421,'0'0'5613,"0"6"-5565,0 15-58,1 49 85,0-66-71,-1 0-1,1 1 0,0-1 1,0 0-1,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,0-1 0,1 1 1,5 5-1,-6-7-1,0-1 0,0 1 1,0-1-1,0 0 0,1 0 0,-1 1 0,0-2 1,1 1-1,-1 0 0,1 0 0,-1-1 0,1 1 1,0-1-1,-1 0 0,1 0 0,-1 0 0,1 0 1,0 0-1,-1-1 0,1 1 0,-1-1 0,1 1 1,-1-1-1,1 0 0,-1 0 0,0 0 0,4-2 1,-1-1-7,1 1 1,-1 0 0,0-1 0,0 0 0,-1 0 0,1-1-1,-1 1 1,0-1 0,0 0 0,3-5 0,-3 2 6,-1 1 0,0-1 0,0 1 0,-1-1-1,0 0 1,0 0 0,-1 0 0,0 0 0,0-13 0,-1 20 74,0 8 161,-3 29-4,-1-1 0,-16 68 0,12-67-148,0 0 0,-3 74 0,11-95-267,-1-8 111,1 0 0,0 0 0,1 0 0,-1-1-1,4 11 1,-4-15-145,1 0 0,-1-1 0,1 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,3-1-1,22 1-5407</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11305.25">4241 343 7764,'0'0'7905,"-5"-1"-7631,5 1-261,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,0 1 0,-1 31 337,2-18-303,0-14-39,0 0 1,0 0-1,0 0 1,1-1-1,-1 1 1,0 0-1,1 0 0,-1 0 1,0 0-1,1 0 1,-1-1-1,1 1 0,-1 0 1,1 0-1,0-1 1,-1 1-1,1 0 1,0-1-1,-1 1 0,1-1 1,0 1-1,0-1 1,-1 1-1,1-1 0,0 1 1,1-1-1,32 6 124,-30-6-117,1 0 0,0 0-1,-1 0 1,1-1 0,-1 1 0,1-1-1,-1-1 1,1 1 0,-1-1 0,0 1-1,8-5 1,-11 5-15,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,-1 0-1,1 0 1,-1-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-2-1 0,-4-2-34,-1 0 0,1 1 0,-1-1 0,1 1 1,-15-3-1,-9 2-15,26 3 38,0 1 0,0-1-1,-1 0 1,1 0 0,0 0 0,0-1-1,-5-2 1,10 4 2,-1 0 0,1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,1-1 0,-1 1-1,0 0 1,0 0 0,0 0 0,0 0 0,1-1 0,-1 1-1,0 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,0-1-1,0 1 1,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,0 0 1,15-8-181,-14 8 162,36-17-380,-5 1 25,1 1 0,1 1 0,0 2 0,51-10-1,-84 22 393,-1 0 1,1 1-1,-1-1 0,0 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1 0 0,-1-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0 25 349,0-20-190,-15 116 1329,17-121-1479,-1-1 0,1 1 0,0-1 0,0 1 0,-1-1 1,1 0-1,0 0 0,0 0 0,0 1 0,-1-2 0,1 1 0,0 0 1,0 0-1,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,2-1 1,-2-2-5,1 0 0,-1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,-1 0 0,1 1 0,-1-1 0,-1-7 1,1 9-11,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 1 0,-1-1 0,1 0 0,-1 1 1,0-1-1,0 1 0,0 0 0,0-1 0,0 1 1,0 0-1,-1 0 0,1 0 0,-1 1 0,1-1 1,-1 1-1,1-1 0,-1 1 0,0 0 0,0 0 1,-3-1-1,5 2-20,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 1 0,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,0 1 0,0 0 1,0-1-1,0 1 0,1 0 1,-1 0-1,0 0 0,0 0 0,1-1 1,-1 1-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 1 1,-1-1-1,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 2 0,-1 3-633,1 0 0,0 0 0,0 1 0,1-1 0,0 0 0,2 9 0,5 2-3721</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11568.33">4893 307 5987,'0'0'12563,"-2"-3"-11982,-4-8-292,49 8-279,59-2-2243,-61 2-1705,70 3 1,-104 4 813,-6 5-3074</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11753.82">5104 364 2273,'0'0'6435,"-117"39"-4114,73-28-208,5 0-160,15-5-721,9-3-127,10-3-321,15 0-784,19 0 0,15 0-64,5-9-1408,4-2-1362,1-3-3200</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12158.03">5755 20 9092,'0'0'6520,"-16"-5"-6186,-53-9-137,66 14-176,1 0-1,-1 1 0,0-1 0,0 1 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 1 0,-1-1 0,1 0 0,0 1 1,0 0-1,-1-1 0,1 1 0,0 0 0,1 0 1,-1 0-1,0 1 0,1-1 0,-1 0 0,1 1 0,-1-1 1,0 3-1,-5 6 132,-3 5-40,1-1 1,1 1-1,0 1 1,1 0 0,1 0-1,0 0 1,2 1-1,-4 20 1,2 11 318,1 88 0,6-127-461,0 0 1,1 0-1,0 0 0,0 0 0,1 0 1,0 0-1,1-1 0,0 1 0,1-1 1,0 0-1,0 0 0,1-1 0,0 0 1,0 0-1,1 0 0,0-1 0,1 0 1,-1 0-1,1-1 0,1 1 0,-1-2 1,1 0-1,0 0 0,0 0 0,0-1 1,1 0-1,0-1 0,0 0 0,0-1 1,0 0-1,0 0 0,13-1 0,-16 0-107,0-1-1,1 0 0,-1-1 0,0 1 1,0-2-1,0 1 0,10-4 0,-15 4 124,0 0 0,0-1-1,-1 1 1,1-1 0,0 1-1,0-1 1,-1 0 0,1 0-1,-1 1 1,1-1-1,-1 0 1,0 0 0,0 0-1,0-1 1,0 1 0,0 0-1,-1 0 1,1-1 0,-1 1-1,1 0 1,-1-1 0,0 1-1,0 0 1,0-1-1,0-4 1,0 1 14,0 0 0,0-1 1,-1 1-1,1 0 0,-2-1 0,1 1 0,-1 0 0,1 0 1,-2 0-1,1 0 0,-1 0 0,0 0 0,0 1 1,0 0-1,-1-1 0,0 1 0,0 0 0,0 1 0,-1-1 1,1 1-1,-1 0 0,0 0 0,0 0 0,-1 1 0,1-1 1,-1 1-1,0 1 0,1-1 0,-1 1 0,-8-2 0,-33-1 62,22 7-1276,24-1 1038,1-1 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 1 1,1-1-1,-1 0 0,1 0 0,0 1 1,-1-1-1,1 0 0,-1 1 1,1-1-1,0 0 0,-1 1 0,1-1 1,0 1-1,-1-1 0,1 0 1,0 1-1,0-1 0,0 1 0,-1-1 1,1 1-1,0 0 0,0 2-2836</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12829.77">6030 279 10981,'0'0'5680,"-20"14"-4856,-63 48-301,80-60-492,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,1 0-1,-1 0 1,1 1 0,0-1 0,-1 0 0,1 0 0,1 0 0,-1 0 0,0 0 0,2 4 0,-1 11 147,-1-16-169,0-1 1,0 0-1,0 0 1,1 0-1,-1 1 0,0-1 1,1 0-1,-1 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 0,0-1 1,0 1-1,0 0 0,0-1 1,0 1-1,2 0 1,0 0 7,1 1 1,0-1 0,0-1 0,-1 1 0,1 0 0,0-1-1,0 0 1,6 0 0,0-1 17,1 0 1,-1-1-1,1 0 1,-1 0-1,16-7 1,-20 6-27,0 0 0,0-1 0,0 0-1,0 0 1,-1 0 0,0-1 0,0 1 0,0-1 0,0-1 0,-1 1 0,0-1-1,0 1 1,0-1 0,-1 0 0,0-1 0,0 1 0,-1 0 0,1-1-1,-2 0 1,1 1 0,0-1 0,-1 0 0,-1 0 0,1 0 0,-1 0-1,0 0 1,-1 0 0,1 1 0,-1-1 0,-3-9 0,2 12-17,1 1 0,-1 0 0,0-1 1,-1 1-1,1 0 0,0 0 0,-1 0 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 0,0 0 1,-1 1-1,1-1 0,-1 0 0,1 1 0,-1 0 1,0 0-1,1 0 0,-1 1 0,0-1 0,0 1 0,0 0 1,0 0-1,-6 1 0,8-1-61,19 0-886,163-13-1977,-115 7 2379,-21 5 455,-43 1 100,-1 0 0,1 1 1,-1-1-1,1 0 0,0 0 1,-1 0-1,1 1 0,-1-1 0,1 0 1,-1 1-1,1-1 0,-1 0 1,1 1-1,-1-1 0,0 0 1,1 1-1,-1-1 0,0 1 1,1-1-1,-1 1 0,0-1 1,1 1-1,-1-1 0,0 1 1,0 0-1,0-1 0,1 1 1,-1-1-1,0 1 0,0-1 1,0 1-1,0 0 0,0 0 1,-1 21 220,1-19-123,-20 129 2486,21-131-2577,-1 1-1,1-1 1,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0 0,1-1 0,-1 1 0,1-1 0,2 1 12,0-1 0,0 0 0,0 1 0,0-2 1,0 1-1,0 0 0,-1-1 0,1 0 0,6-4 0,-5 1-10,0-1-1,-1-1 1,0 1-1,0-1 0,-1 1 1,0-1-1,0 0 1,0-1-1,-1 1 1,0 0-1,-1-1 1,1 1-1,-2-1 1,1 1-1,-1-14 1,0 18-7,0-1 0,0 1 1,-1-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,0 1 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,-1 0-1,1 1 1,-1-1-1,1 1 0,-1-1 1,0 1-1,1 0 1,-1 0-1,0 1 1,-1-1-1,1 0 0,0 1 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 1 1,-7-1-1,0 1-132,-1 0 1,1 1-1,0 0 0,-1 1 1,1 0-1,0 1 0,0 0 0,0 0 1,0 1-1,1 0 0,-1 1 1,1 0-1,0 0 0,-14 12 0,-4 6-2932</inkml:trace>
-</inkml:ink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1613,7 +1334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:P1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
@@ -1625,7 +1346,7 @@
   <sheetData>
     <row r="1" spans="3:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="39" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="27"/>
@@ -1660,7 +1381,7 @@
     </row>
     <row r="6" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="7" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="38" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="36"/>
@@ -1683,7 +1404,7 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="26" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="27"/>
@@ -1766,7 +1487,7 @@
     </row>
     <row r="14" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="15" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="38" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="36"/>
@@ -1788,7 +1509,7 @@
       <c r="C17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="40" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="36"/>
@@ -1801,7 +1522,7 @@
       <c r="C18" s="3">
         <v>1</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="35" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="36"/>
@@ -1814,7 +1535,7 @@
       <c r="C19" s="3">
         <v>2</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="36"/>
@@ -1827,7 +1548,7 @@
       <c r="C20" s="3">
         <v>3</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="35" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="36"/>
@@ -1840,7 +1561,7 @@
       <c r="C21" s="3">
         <v>4</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="35" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="36"/>
@@ -1853,7 +1574,7 @@
       <c r="C22" s="3">
         <v>5</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="35" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="36"/>
@@ -1866,7 +1587,7 @@
       <c r="C23" s="3">
         <v>6</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="35" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="36"/>
@@ -1879,7 +1600,7 @@
       <c r="C24" s="3">
         <v>7</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="35" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="36"/>
@@ -1892,7 +1613,7 @@
       <c r="C25" s="3">
         <v>8</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="35" t="s">
         <v>13</v>
       </c>
       <c r="E25" s="36"/>
@@ -1905,7 +1626,7 @@
       <c r="C26" s="3">
         <v>9</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="35" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="36"/>
@@ -1918,7 +1639,7 @@
       <c r="C27" s="3">
         <v>10</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="35" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="36"/>
@@ -1931,7 +1652,7 @@
       <c r="C28" s="3">
         <v>11</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="35" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="36"/>
@@ -1944,7 +1665,7 @@
       <c r="C29" s="3">
         <v>12</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="35" t="s">
         <v>17</v>
       </c>
       <c r="E29" s="36"/>
@@ -1957,7 +1678,7 @@
       <c r="C30" s="3">
         <v>13</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="35" t="s">
         <v>18</v>
       </c>
       <c r="E30" s="36"/>
@@ -1970,7 +1691,7 @@
       <c r="C31" s="3">
         <v>14</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="35" t="s">
         <v>19</v>
       </c>
       <c r="E31" s="36"/>
@@ -1983,7 +1704,7 @@
       <c r="C32" s="3">
         <v>15</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="35" t="s">
         <v>20</v>
       </c>
       <c r="E32" s="36"/>
@@ -1996,7 +1717,7 @@
       <c r="C33" s="3">
         <v>16</v>
       </c>
-      <c r="D33" s="40" t="s">
+      <c r="D33" s="35" t="s">
         <v>21</v>
       </c>
       <c r="E33" s="36"/>
@@ -2009,7 +1730,7 @@
       <c r="C34" s="3">
         <v>17</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="35" t="s">
         <v>22</v>
       </c>
       <c r="E34" s="36"/>
@@ -2022,7 +1743,7 @@
       <c r="C35" s="3">
         <v>18</v>
       </c>
-      <c r="D35" s="40" t="s">
+      <c r="D35" s="35" t="s">
         <v>23</v>
       </c>
       <c r="E35" s="36"/>
@@ -2035,7 +1756,7 @@
       <c r="C36" s="3">
         <v>19</v>
       </c>
-      <c r="D36" s="40" t="s">
+      <c r="D36" s="35" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="36"/>
@@ -2048,7 +1769,7 @@
       <c r="C37" s="3">
         <v>20</v>
       </c>
-      <c r="D37" s="40" t="s">
+      <c r="D37" s="35" t="s">
         <v>25</v>
       </c>
       <c r="E37" s="36"/>
@@ -2061,7 +1782,7 @@
       <c r="C38" s="3">
         <v>21</v>
       </c>
-      <c r="D38" s="40" t="s">
+      <c r="D38" s="35" t="s">
         <v>26</v>
       </c>
       <c r="E38" s="36"/>
@@ -2073,7 +1794,7 @@
     <row r="39" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="40" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="41" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="38" t="s">
         <v>27</v>
       </c>
       <c r="D41" s="36"/>
@@ -2092,7 +1813,7 @@
     </row>
     <row r="42" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="43" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C43" s="38" t="s">
+      <c r="C43" s="26" t="s">
         <v>28</v>
       </c>
       <c r="D43" s="27"/>
@@ -3128,6 +2849,21 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="G2:L5"/>
+    <mergeCell ref="C7:P7"/>
+    <mergeCell ref="C9:P13"/>
+    <mergeCell ref="C15:P15"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="D18:I18"/>
+    <mergeCell ref="D19:I19"/>
+    <mergeCell ref="D20:I20"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="D22:I22"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="D25:I25"/>
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="D34:I34"/>
     <mergeCell ref="C43:P47"/>
     <mergeCell ref="D27:I27"/>
     <mergeCell ref="D28:I28"/>
@@ -3141,21 +2877,6 @@
     <mergeCell ref="D37:I37"/>
     <mergeCell ref="D38:I38"/>
     <mergeCell ref="C41:P41"/>
-    <mergeCell ref="D23:I23"/>
-    <mergeCell ref="D24:I24"/>
-    <mergeCell ref="D25:I25"/>
-    <mergeCell ref="D26:I26"/>
-    <mergeCell ref="D34:I34"/>
-    <mergeCell ref="D18:I18"/>
-    <mergeCell ref="D19:I19"/>
-    <mergeCell ref="D20:I20"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="D22:I22"/>
-    <mergeCell ref="G2:L5"/>
-    <mergeCell ref="C7:P7"/>
-    <mergeCell ref="C9:P13"/>
-    <mergeCell ref="C15:P15"/>
-    <mergeCell ref="D17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -4281,7 +4002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="C1:I1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
@@ -5407,8 +5128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C1:I1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5496,22 +5217,30 @@
     <row r="14" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="15" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="16" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="17" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D17" s="47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D18" s="48">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="20" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="21" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="22" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="24" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="28" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="29" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="30" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="31" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="32" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7602,8 +7331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:H1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -11784,7 +11513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C1:I1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
@@ -18854,7 +18583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:H1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>